<commit_message>
Bug fixes with animation, smoothed out animation Bug fixes with AI/pathing
</commit_message>
<xml_diff>
--- a/assets/dataSet.xlsx
+++ b/assets/dataSet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Map 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="20">
   <si>
     <t xml:space="preserve">X19</t>
   </si>
@@ -74,16 +74,13 @@
     <t xml:space="preserve">X24</t>
   </si>
   <si>
-    <t xml:space="preserve">.1</t>
+    <t xml:space="preserve">T1</t>
   </si>
   <si>
-    <t xml:space="preserve">.3</t>
+    <t xml:space="preserve">T4</t>
   </si>
   <si>
-    <t xml:space="preserve">.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.4</t>
+    <t xml:space="preserve">T4B</t>
   </si>
 </sst>
 </file>
@@ -93,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -114,6 +111,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,12 +160,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,8 +192,8 @@
   </sheetPr>
   <dimension ref="A2:AA21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="0" sqref="O16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1579,8 +1585,8 @@
   </sheetPr>
   <dimension ref="A2:T33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T21" activeCellId="0" sqref="T21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1592,203 +1598,203 @@
       <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
+      <c r="E5" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
@@ -1806,7 +1812,7 @@
         <v>7</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>7</v>
@@ -1833,12 +1839,12 @@
         <v>7</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1892,21 +1898,21 @@
         <v>7</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -1933,7 +1939,7 @@
         <v>7</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>7</v>
@@ -1948,7 +1954,7 @@
         <v>7</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>7</v>
@@ -1957,12 +1963,12 @@
         <v>7</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -1980,10 +1986,10 @@
         <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>7</v>
@@ -2004,7 +2010,7 @@
         <v>7</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>7</v>
@@ -2019,12 +2025,12 @@
         <v>7</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -2042,10 +2048,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>7</v>
@@ -2069,7 +2075,7 @@
         <v>7</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>7</v>
@@ -2081,12 +2087,12 @@
         <v>7</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -2122,19 +2128,19 @@
         <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>7</v>
@@ -2143,21 +2149,21 @@
         <v>7</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>7</v>
@@ -2178,7 +2184,7 @@
         <v>7</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>7</v>
@@ -2187,16 +2193,16 @@
         <v>7</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>7</v>
@@ -2205,12 +2211,12 @@
         <v>7</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
@@ -2219,7 +2225,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
@@ -2255,7 +2261,7 @@
         <v>7</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>7</v>
@@ -2264,15 +2270,15 @@
         <v>7</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -2329,12 +2335,12 @@
         <v>7</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -2391,15 +2397,15 @@
         <v>7</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -2447,30 +2453,30 @@
         <v>7</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>7</v>
@@ -2482,7 +2488,7 @@
         <v>7</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>7</v>
@@ -2515,21 +2521,21 @@
         <v>7</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
@@ -2547,7 +2553,7 @@
         <v>7</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>7</v>
@@ -2562,7 +2568,7 @@
         <v>7</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="P17" s="1" t="s">
         <v>7</v>
@@ -2571,18 +2577,18 @@
         <v>7</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
@@ -2609,7 +2615,7 @@
         <v>7</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>7</v>
@@ -2618,7 +2624,7 @@
         <v>7</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>7</v>
@@ -2635,16 +2641,16 @@
       <c r="R18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>7</v>
+      <c r="S18" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -2659,7 +2665,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
@@ -2686,7 +2692,7 @@
         <v>7</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>7</v>
@@ -2695,18 +2701,18 @@
         <v>7</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
@@ -2760,72 +2766,72 @@
         <v>7</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="P21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="R21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="S21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="T21" s="0" t="s">
-        <v>16</v>
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>